<commit_message>
done round.vhd and countern.vhd
</commit_message>
<xml_diff>
--- a/PARTE_SECONDA/NPU_blocks.xlsx
+++ b/PARTE_SECONDA/NPU_blocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\LibriUniversitari\GitHub\Workshop_Innovative_Systems\PARTE_SECONDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72835C7D-3B27-4A71-B870-C80A9780267D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C8EB59-C00D-41CB-B083-CCED3B405ED7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>VHDL file</t>
   </si>
@@ -87,18 +87,28 @@
     <t>dp.vhd</t>
   </si>
   <si>
-    <t>Synchronous counter with generic paralleism,  asynchronous reset,  enable signal, synchronous clear and programmable terminal count.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(@cnt.m) + (@muxnto1_nbit.m)(synch clear) + (@add_sub + @or + @norn)(programmable tc)
+    <t xml:space="preserve">(@cnt.m) + (@muxnto1_nbit.m)(synch clear) + (@add_sub + @or + @(norn)(programmable tc)
 </t>
+  </si>
+  <si>
+    <t>✔</t>
+  </si>
+  <si>
+    <t>Synchronous counter with generic parallelism,  asynchronous reset,  enable signal, synchronous clear and programmable terminal count.</t>
+  </si>
+  <si>
+    <t>Combinational logic capable of performing rounding to nearest even,
+ the input and output parallelism is generic.</t>
+  </si>
+  <si>
+    <t>(@rca.m) +  3*(@muxnto1_nbit.m) + (@orn)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +118,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -160,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -183,6 +201,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,13 +493,13 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" style="3" customWidth="1"/>
-    <col min="3" max="3" width="59.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="78.5546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="60" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -501,9 +522,12 @@
         <v>4</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -512,9 +536,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -556,6 +589,7 @@
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">

</xml_diff>

<commit_message>
done relu, round and pool
</commit_message>
<xml_diff>
--- a/PARTE_SECONDA/NPU_blocks.xlsx
+++ b/PARTE_SECONDA/NPU_blocks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\Documents\GitHub\Workshop_Innovative_Systems\PARTE_SECONDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\LibriUniversitari\GitHub\Workshop_Innovative_Systems\PARTE_SECONDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72300FB-F6E2-4F3C-B843-44467A02CBF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83B1E78-688D-4947-8CF2-E8D192B118A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>VHDL file</t>
   </si>
@@ -101,13 +101,28 @@
  the input and output parallelism is generic.</t>
   </si>
   <si>
-    <t>(@rca.m) +  3*(@muxnto1_nbit.m) + (@orn)</t>
-  </si>
-  <si>
     <t>Sequential circuit capable of providing the correct address</t>
   </si>
   <si>
     <t>4*(@rca.m) +  5*(@muxnto1_nbit.m) + (@or2) + 2*(@flip_flop)</t>
+  </si>
+  <si>
+    <t>(@rca.m) +  3*(@muxnto1_nbit.m) + (@orn.m)</t>
+  </si>
+  <si>
+    <t>Combinational logic capable of performing a quantization,
+ the input and output parallelism is generic.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(@orn.m) + 3*(@nand.m) + (@nor.m) + n_O*(@muxnto1_nbit.m) </t>
+  </si>
+  <si>
+    <t>Sequential circuit that performs the sum of four quantities in
+three clock cycle, the data width is generic.</t>
+  </si>
+  <si>
+    <t>(@rca.m)(N+1) + (@rca.m)(N+2) + 2*(@register.m)(N+1) +
++ (@register.m)(N+1) + 3*(@muxnto1_nbit.m)</t>
   </si>
 </sst>
 </file>
@@ -184,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -209,6 +224,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -498,18 +519,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" style="3" customWidth="1"/>
-    <col min="3" max="3" width="78.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="78.5546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="60" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -523,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -537,21 +558,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
@@ -559,74 +580,93 @@
         <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="C13" s="11"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>